<commit_message>
update something idk my wife left me
</commit_message>
<xml_diff>
--- a/Coursework Reports/5th assignment/xlsx5.xlsx
+++ b/Coursework Reports/5th assignment/xlsx5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D21159-7A8C-460E-A4AC-BCCABFEDBE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1273C302-5BAE-49B6-AA7B-0BCD0CC3C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6934,8 +6934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>